<commit_message>
adding correct info to standings
Signed-off-by: YelloElefant <alextrotternz@gmail.com>
</commit_message>
<xml_diff>
--- a/Assets/u15tournamentwebsitestuff/2023 U15 Draw & Venues.xlsx
+++ b/Assets/u15tournamentwebsitestuff/2023 U15 Draw & Venues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewh/Desktop/bits n bobs /U15 Torneo 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/Assets/u15tournamentwebsitestuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242B7690-5CB0-5A45-A391-BF1C8606AF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="27640" windowHeight="15680" xr2:uid="{42E46D64-C3F8-9247-A5C1-B0B9AA97A173}"/>
+    <workbookView minimized="1" xWindow="-21600" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{42E46D64-C3F8-9247-A5C1-B0B9AA97A173}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1278,26 +1278,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CFDC66-E60D-C246-898B-7879750985C3}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36.5" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="36.5" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.375" style="6" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="1"/>
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>9</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>10</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>11</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>12</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>13</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>15</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -1849,7 +1849,7 @@
       <c r="I19" s="58"/>
       <c r="J19" s="59"/>
     </row>
-    <row r="20" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="1"/>
@@ -1861,7 +1861,7 @@
       <c r="I20" s="58"/>
       <c r="J20" s="58"/>
     </row>
-    <row r="21" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +1883,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>17</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>18</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="J23" s="61"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>19</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>20</v>
       </c>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>21</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>22</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>23</v>
       </c>
@@ -2068,7 +2068,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>24</v>
       </c>
@@ -2093,7 +2093,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="1"/>
@@ -2104,7 +2104,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>1</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>25</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>26</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>27</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>28</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>29</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>30</v>
       </c>
@@ -2267,7 +2267,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>31</v>
       </c>
@@ -2290,7 +2290,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>32</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="37"/>
       <c r="C40" s="1"/>
@@ -2324,7 +2324,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>1</v>
       </c>
@@ -2345,7 +2345,7 @@
       <c r="H41" s="9"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>33</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>34</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>35</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>36</v>
       </c>
@@ -2441,7 +2441,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>37</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>38</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>39</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>40</v>
       </c>
@@ -2537,7 +2537,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="37"/>
       <c r="C50" s="1"/>
@@ -2548,7 +2548,7 @@
       <c r="H50" s="5"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>1</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>41</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="H52" s="7"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>42</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>43</v>
       </c>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>44</v>
       </c>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>45</v>
       </c>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>46</v>
       </c>
@@ -2725,7 +2725,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>47</v>
       </c>
@@ -2750,7 +2750,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>48</v>
       </c>
@@ -2785,6 +2785,6 @@
     <mergeCell ref="C41:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>